<commit_message>
final edits to code annotation and final paper
</commit_message>
<xml_diff>
--- a/Research_Assignment/fred corporate profit.xlsx
+++ b/Research_Assignment/fred corporate profit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tklein/Desktop/JHU_Classes/computational_modeling/Research_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6798480C-1EBB-0E4C-9053-E6093D8698A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7B093B3D-4E51-064E-8BDD-F58B6C1867A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
   </bookViews>
@@ -9584,9 +9584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>